<commit_message>
intro of xaml files
</commit_message>
<xml_diff>
--- a/Requests/Request.xlsx
+++ b/Requests/Request.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Robotic_Automation\Requests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Robotic_Automation\Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66181C12-1071-44FD-ACB9-00A907C9A79B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{062AA626-8E2F-417F-B892-3027FBB581DD}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -42,20 +41,31 @@
     <t>Subject</t>
   </si>
   <si>
-    <t>Data Labels</t>
-  </si>
-  <si>
-    <t>Data for support</t>
+    <t>Charles Muli</t>
+  </si>
+  <si>
+    <t>cmcharels.muli@gmail.com</t>
+  </si>
+  <si>
+    <t>registration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,13 +88,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -396,42 +409,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4795D496-ACC7-4361-A8D2-08954DB7EBF6}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter>
     <oddFooter>&amp;R&amp;1#&amp;"Calibri"&amp;10&amp;K000000C1 - Public</oddFooter>
   </headerFooter>

</xml_diff>